<commit_message>
Future score heuristic, added deploy stat for card
</commit_message>
<xml_diff>
--- a/TUnderdark/Resources/Cards.xlsx
+++ b/TUnderdark/Resources/Cards.xlsx
@@ -9,20 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12885"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cards!$A$1:$G$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cards!$A$1:$N$126</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="291">
   <si>
     <t>SpecificType</t>
   </si>
@@ -892,6 +892,9 @@
   </si>
   <si>
     <t>DrawSpeed</t>
+  </si>
+  <si>
+    <t>Deploy</t>
   </si>
 </sst>
 </file>
@@ -1206,11 +1209,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M126"/>
+  <dimension ref="A1:N126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L108" sqref="L108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,7 +1230,7 @@
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1267,8 +1270,11 @@
       <c r="M1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1308,8 +1314,11 @@
       <c r="M2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1349,8 +1358,11 @@
       <c r="M3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1390,8 +1402,11 @@
       <c r="M4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1431,8 +1446,11 @@
       <c r="M5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1472,8 +1490,11 @@
       <c r="M6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1513,8 +1534,11 @@
       <c r="M7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1554,8 +1578,11 @@
       <c r="M8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1595,8 +1622,11 @@
       <c r="M9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1636,8 +1666,11 @@
       <c r="M10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1677,8 +1710,11 @@
       <c r="M11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1718,8 +1754,11 @@
       <c r="M12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1759,8 +1798,11 @@
       <c r="M13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1800,8 +1842,11 @@
       <c r="M14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1841,8 +1886,11 @@
       <c r="M15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1882,8 +1930,11 @@
       <c r="M16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1923,8 +1974,11 @@
       <c r="M17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1964,8 +2018,11 @@
       <c r="M18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2005,8 +2062,11 @@
       <c r="M19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2046,8 +2106,11 @@
       <c r="M20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2087,8 +2150,11 @@
       <c r="M21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2128,8 +2194,11 @@
       <c r="M22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2169,8 +2238,11 @@
       <c r="M23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -2210,8 +2282,11 @@
       <c r="M24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2251,8 +2326,11 @@
       <c r="M25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2292,8 +2370,11 @@
       <c r="M26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -2333,8 +2414,11 @@
       <c r="M27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -2374,8 +2458,11 @@
       <c r="M28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -2415,8 +2502,11 @@
       <c r="M29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -2456,8 +2546,11 @@
       <c r="M30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -2497,8 +2590,11 @@
       <c r="M31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2538,8 +2634,11 @@
       <c r="M32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -2579,8 +2678,11 @@
       <c r="M33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2620,8 +2722,11 @@
       <c r="M34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -2661,8 +2766,11 @@
       <c r="M35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2702,8 +2810,11 @@
       <c r="M36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -2743,8 +2854,11 @@
       <c r="M37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2784,8 +2898,11 @@
       <c r="M38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>92</v>
       </c>
@@ -2825,8 +2942,11 @@
       <c r="M39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -2866,8 +2986,11 @@
       <c r="M40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -2907,8 +3030,11 @@
       <c r="M41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -2948,8 +3074,11 @@
       <c r="M42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -2989,8 +3118,11 @@
       <c r="M43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>102</v>
       </c>
@@ -3030,8 +3162,11 @@
       <c r="M44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -3071,8 +3206,11 @@
       <c r="M45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>106</v>
       </c>
@@ -3112,8 +3250,11 @@
       <c r="M46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N46">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -3153,8 +3294,11 @@
       <c r="M47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -3194,8 +3338,11 @@
       <c r="M48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -3235,8 +3382,11 @@
       <c r="M49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>115</v>
       </c>
@@ -3276,8 +3426,11 @@
       <c r="M50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>117</v>
       </c>
@@ -3317,8 +3470,11 @@
       <c r="M51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -3358,8 +3514,11 @@
       <c r="M52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>121</v>
       </c>
@@ -3399,8 +3558,11 @@
       <c r="M53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>124</v>
       </c>
@@ -3440,8 +3602,11 @@
       <c r="M54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N54">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>126</v>
       </c>
@@ -3481,8 +3646,11 @@
       <c r="M55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>128</v>
       </c>
@@ -3522,8 +3690,11 @@
       <c r="M56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>130</v>
       </c>
@@ -3563,8 +3734,11 @@
       <c r="M57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N57">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>133</v>
       </c>
@@ -3604,8 +3778,11 @@
       <c r="M58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>135</v>
       </c>
@@ -3645,8 +3822,11 @@
       <c r="M59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>137</v>
       </c>
@@ -3686,8 +3866,11 @@
       <c r="M60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N60">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>139</v>
       </c>
@@ -3727,8 +3910,11 @@
       <c r="M61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>141</v>
       </c>
@@ -3768,8 +3954,11 @@
       <c r="M62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N62">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>143</v>
       </c>
@@ -3809,8 +3998,11 @@
       <c r="M63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>145</v>
       </c>
@@ -3850,8 +4042,11 @@
       <c r="M64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>147</v>
       </c>
@@ -3891,8 +4086,11 @@
       <c r="M65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -3932,8 +4130,11 @@
       <c r="M66">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>152</v>
       </c>
@@ -3973,8 +4174,11 @@
       <c r="M67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>154</v>
       </c>
@@ -4014,8 +4218,11 @@
       <c r="M68">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>156</v>
       </c>
@@ -4055,8 +4262,11 @@
       <c r="M69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N69">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>158</v>
       </c>
@@ -4096,8 +4306,11 @@
       <c r="M70">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>160</v>
       </c>
@@ -4137,8 +4350,11 @@
       <c r="M71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>162</v>
       </c>
@@ -4178,8 +4394,11 @@
       <c r="M72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>164</v>
       </c>
@@ -4219,8 +4438,11 @@
       <c r="M73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>166</v>
       </c>
@@ -4260,8 +4482,11 @@
       <c r="M74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>168</v>
       </c>
@@ -4301,8 +4526,11 @@
       <c r="M75">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>171</v>
       </c>
@@ -4342,8 +4570,11 @@
       <c r="M76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>174</v>
       </c>
@@ -4383,8 +4614,11 @@
       <c r="M77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>177</v>
       </c>
@@ -4424,8 +4658,11 @@
       <c r="M78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>179</v>
       </c>
@@ -4465,8 +4702,11 @@
       <c r="M79">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>181</v>
       </c>
@@ -4506,8 +4746,11 @@
       <c r="M80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>183</v>
       </c>
@@ -4547,8 +4790,11 @@
       <c r="M81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>185</v>
       </c>
@@ -4588,8 +4834,11 @@
       <c r="M82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>188</v>
       </c>
@@ -4629,8 +4878,11 @@
       <c r="M83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N83">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>190</v>
       </c>
@@ -4670,8 +4922,11 @@
       <c r="M84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>192</v>
       </c>
@@ -4711,8 +4966,11 @@
       <c r="M85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N85">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>194</v>
       </c>
@@ -4752,8 +5010,11 @@
       <c r="M86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>196</v>
       </c>
@@ -4793,8 +5054,11 @@
       <c r="M87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>199</v>
       </c>
@@ -4834,8 +5098,11 @@
       <c r="M88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N88">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>201</v>
       </c>
@@ -4875,8 +5142,11 @@
       <c r="M89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>204</v>
       </c>
@@ -4916,8 +5186,11 @@
       <c r="M90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>206</v>
       </c>
@@ -4957,8 +5230,11 @@
       <c r="M91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>209</v>
       </c>
@@ -4998,8 +5274,11 @@
       <c r="M92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>212</v>
       </c>
@@ -5039,8 +5318,11 @@
       <c r="M93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>214</v>
       </c>
@@ -5080,8 +5362,11 @@
       <c r="M94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>216</v>
       </c>
@@ -5121,8 +5406,11 @@
       <c r="M95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>219</v>
       </c>
@@ -5162,8 +5450,11 @@
       <c r="M96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>222</v>
       </c>
@@ -5203,8 +5494,11 @@
       <c r="M97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>224</v>
       </c>
@@ -5244,8 +5538,11 @@
       <c r="M98">
         <v>2</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>226</v>
       </c>
@@ -5285,8 +5582,11 @@
       <c r="M99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>228</v>
       </c>
@@ -5326,8 +5626,11 @@
       <c r="M100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>230</v>
       </c>
@@ -5367,8 +5670,11 @@
       <c r="M101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>232</v>
       </c>
@@ -5408,8 +5714,11 @@
       <c r="M102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N102">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>234</v>
       </c>
@@ -5449,8 +5758,11 @@
       <c r="M103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>236</v>
       </c>
@@ -5490,8 +5802,11 @@
       <c r="M104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>238</v>
       </c>
@@ -5531,8 +5846,11 @@
       <c r="M105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>240</v>
       </c>
@@ -5572,8 +5890,11 @@
       <c r="M106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>243</v>
       </c>
@@ -5613,8 +5934,11 @@
       <c r="M107">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>245</v>
       </c>
@@ -5654,8 +5978,11 @@
       <c r="M108">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>247</v>
       </c>
@@ -5695,8 +6022,11 @@
       <c r="M109">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N109">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>249</v>
       </c>
@@ -5736,8 +6066,11 @@
       <c r="M110">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>251</v>
       </c>
@@ -5777,8 +6110,11 @@
       <c r="M111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>253</v>
       </c>
@@ -5818,8 +6154,11 @@
       <c r="M112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N112">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>256</v>
       </c>
@@ -5859,8 +6198,11 @@
       <c r="M113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>258</v>
       </c>
@@ -5900,8 +6242,11 @@
       <c r="M114">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>260</v>
       </c>
@@ -5941,8 +6286,11 @@
       <c r="M115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>262</v>
       </c>
@@ -5982,8 +6330,11 @@
       <c r="M116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>264</v>
       </c>
@@ -6023,8 +6374,11 @@
       <c r="M117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>266</v>
       </c>
@@ -6064,8 +6418,11 @@
       <c r="M118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>268</v>
       </c>
@@ -6105,8 +6462,11 @@
       <c r="M119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>270</v>
       </c>
@@ -6146,8 +6506,11 @@
       <c r="M120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>272</v>
       </c>
@@ -6187,8 +6550,11 @@
       <c r="M121">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>274</v>
       </c>
@@ -6228,8 +6594,11 @@
       <c r="M122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>276</v>
       </c>
@@ -6269,8 +6638,11 @@
       <c r="M123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N123">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>278</v>
       </c>
@@ -6310,8 +6682,11 @@
       <c r="M124">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N124">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>280</v>
       </c>
@@ -6351,8 +6726,11 @@
       <c r="M125">
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N125">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>282</v>
       </c>
@@ -6392,8 +6770,12 @@
       <c r="M126">
         <v>0</v>
       </c>
+      <c r="N126">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N126"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Future value from cities
</commit_message>
<xml_diff>
--- a/TUnderdark/Resources/Cards.xlsx
+++ b/TUnderdark/Resources/Cards.xlsx
@@ -1212,8 +1212,8 @@
   <dimension ref="A1:N126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L108" sqref="L108"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Return enemy spies card stats
</commit_message>
<xml_diff>
--- a/TUnderdark/Resources/Cards.xlsx
+++ b/TUnderdark/Resources/Cards.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="27870" windowHeight="12885"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="292">
   <si>
     <t>SpecificType</t>
   </si>
@@ -895,6 +895,9 @@
   </si>
   <si>
     <t>Deploy</t>
+  </si>
+  <si>
+    <t>ReturnEnemySpy</t>
   </si>
 </sst>
 </file>
@@ -1209,11 +1212,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N126"/>
+  <dimension ref="A1:O126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N126" sqref="N126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,7 +1233,7 @@
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1273,8 +1276,11 @@
       <c r="N1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1317,8 +1323,11 @@
       <c r="N2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1361,8 +1370,11 @@
       <c r="N3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1405,8 +1417,11 @@
       <c r="N4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1449,8 +1464,11 @@
       <c r="N5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1493,8 +1511,11 @@
       <c r="N6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1537,8 +1558,11 @@
       <c r="N7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1581,8 +1605,11 @@
       <c r="N8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1625,8 +1652,11 @@
       <c r="N9">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1669,8 +1699,11 @@
       <c r="N10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1713,8 +1746,11 @@
       <c r="N11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1757,8 +1793,11 @@
       <c r="N12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1801,8 +1840,11 @@
       <c r="N13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1845,8 +1887,11 @@
       <c r="N14">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1889,8 +1934,11 @@
       <c r="N15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1933,8 +1981,11 @@
       <c r="N16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1977,8 +2028,11 @@
       <c r="N17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -2021,8 +2075,11 @@
       <c r="N18">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2065,8 +2122,11 @@
       <c r="N19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2109,8 +2169,11 @@
       <c r="N20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2153,8 +2216,11 @@
       <c r="N21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2197,8 +2263,11 @@
       <c r="N22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2241,8 +2310,11 @@
       <c r="N23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -2285,8 +2357,11 @@
       <c r="N24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2329,8 +2404,11 @@
       <c r="N25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2373,8 +2451,11 @@
       <c r="N26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -2417,8 +2498,11 @@
       <c r="N27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -2461,8 +2545,11 @@
       <c r="N28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -2505,8 +2592,11 @@
       <c r="N29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -2549,8 +2639,11 @@
       <c r="N30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -2593,8 +2686,11 @@
       <c r="N31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2637,8 +2733,11 @@
       <c r="N32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -2681,8 +2780,11 @@
       <c r="N33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2725,8 +2827,11 @@
       <c r="N34">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -2769,8 +2874,11 @@
       <c r="N35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2813,8 +2921,11 @@
       <c r="N36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -2857,8 +2968,11 @@
       <c r="N37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -2901,8 +3015,11 @@
       <c r="N38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>92</v>
       </c>
@@ -2945,8 +3062,11 @@
       <c r="N39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -2989,8 +3109,11 @@
       <c r="N40">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -3033,8 +3156,11 @@
       <c r="N41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -3077,8 +3203,11 @@
       <c r="N42">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -3121,8 +3250,11 @@
       <c r="N43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>102</v>
       </c>
@@ -3165,8 +3297,11 @@
       <c r="N44">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -3209,8 +3344,11 @@
       <c r="N45">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>106</v>
       </c>
@@ -3253,8 +3391,11 @@
       <c r="N46">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -3297,8 +3438,11 @@
       <c r="N47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -3341,8 +3485,11 @@
       <c r="N48">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -3385,8 +3532,11 @@
       <c r="N49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>115</v>
       </c>
@@ -3429,8 +3579,11 @@
       <c r="N50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>117</v>
       </c>
@@ -3473,8 +3626,11 @@
       <c r="N51">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -3517,8 +3673,11 @@
       <c r="N52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>121</v>
       </c>
@@ -3561,8 +3720,11 @@
       <c r="N53">
         <v>3</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>124</v>
       </c>
@@ -3605,8 +3767,11 @@
       <c r="N54">
         <v>5</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>126</v>
       </c>
@@ -3649,8 +3814,11 @@
       <c r="N55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>128</v>
       </c>
@@ -3693,8 +3861,11 @@
       <c r="N56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>130</v>
       </c>
@@ -3737,8 +3908,11 @@
       <c r="N57">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>133</v>
       </c>
@@ -3781,8 +3955,11 @@
       <c r="N58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>135</v>
       </c>
@@ -3825,8 +4002,11 @@
       <c r="N59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>137</v>
       </c>
@@ -3869,8 +4049,11 @@
       <c r="N60">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>139</v>
       </c>
@@ -3913,8 +4096,11 @@
       <c r="N61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>141</v>
       </c>
@@ -3957,8 +4143,11 @@
       <c r="N62">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>143</v>
       </c>
@@ -4001,8 +4190,11 @@
       <c r="N63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>145</v>
       </c>
@@ -4045,8 +4237,11 @@
       <c r="N64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>147</v>
       </c>
@@ -4089,8 +4284,11 @@
       <c r="N65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -4133,8 +4331,11 @@
       <c r="N66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>152</v>
       </c>
@@ -4177,8 +4378,11 @@
       <c r="N67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>154</v>
       </c>
@@ -4221,8 +4425,11 @@
       <c r="N68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O68">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>156</v>
       </c>
@@ -4265,8 +4472,11 @@
       <c r="N69">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O69">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>158</v>
       </c>
@@ -4309,8 +4519,11 @@
       <c r="N70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>160</v>
       </c>
@@ -4353,8 +4566,11 @@
       <c r="N71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>162</v>
       </c>
@@ -4397,8 +4613,11 @@
       <c r="N72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>164</v>
       </c>
@@ -4441,8 +4660,11 @@
       <c r="N73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>166</v>
       </c>
@@ -4485,8 +4707,11 @@
       <c r="N74">
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>168</v>
       </c>
@@ -4529,8 +4754,11 @@
       <c r="N75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O75">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>171</v>
       </c>
@@ -4573,8 +4801,11 @@
       <c r="N76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>174</v>
       </c>
@@ -4617,8 +4848,11 @@
       <c r="N77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>177</v>
       </c>
@@ -4661,8 +4895,11 @@
       <c r="N78">
         <v>2</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O78">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>179</v>
       </c>
@@ -4705,8 +4942,11 @@
       <c r="N79">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>181</v>
       </c>
@@ -4749,8 +4989,11 @@
       <c r="N80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>183</v>
       </c>
@@ -4793,8 +5036,11 @@
       <c r="N81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>185</v>
       </c>
@@ -4837,8 +5083,11 @@
       <c r="N82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>188</v>
       </c>
@@ -4881,8 +5130,11 @@
       <c r="N83">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O83">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>190</v>
       </c>
@@ -4925,8 +5177,11 @@
       <c r="N84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>192</v>
       </c>
@@ -4969,8 +5224,11 @@
       <c r="N85">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>194</v>
       </c>
@@ -5013,8 +5271,11 @@
       <c r="N86">
         <v>2</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O86">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>196</v>
       </c>
@@ -5057,8 +5318,11 @@
       <c r="N87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O87">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>199</v>
       </c>
@@ -5101,8 +5365,11 @@
       <c r="N88">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>201</v>
       </c>
@@ -5145,8 +5412,11 @@
       <c r="N89">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O89">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>204</v>
       </c>
@@ -5189,8 +5459,11 @@
       <c r="N90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>206</v>
       </c>
@@ -5233,8 +5506,11 @@
       <c r="N91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>209</v>
       </c>
@@ -5277,8 +5553,11 @@
       <c r="N92">
         <v>3</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>212</v>
       </c>
@@ -5321,8 +5600,11 @@
       <c r="N93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>214</v>
       </c>
@@ -5365,8 +5647,11 @@
       <c r="N94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>216</v>
       </c>
@@ -5409,8 +5694,11 @@
       <c r="N95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>219</v>
       </c>
@@ -5453,8 +5741,11 @@
       <c r="N96">
         <v>2</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>222</v>
       </c>
@@ -5497,8 +5788,11 @@
       <c r="N97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>224</v>
       </c>
@@ -5541,8 +5835,11 @@
       <c r="N98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>226</v>
       </c>
@@ -5585,8 +5882,11 @@
       <c r="N99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>228</v>
       </c>
@@ -5629,8 +5929,11 @@
       <c r="N100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>230</v>
       </c>
@@ -5673,8 +5976,11 @@
       <c r="N101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>232</v>
       </c>
@@ -5717,8 +6023,11 @@
       <c r="N102">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O102">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>234</v>
       </c>
@@ -5761,8 +6070,11 @@
       <c r="N103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>236</v>
       </c>
@@ -5805,8 +6117,11 @@
       <c r="N104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>238</v>
       </c>
@@ -5849,8 +6164,11 @@
       <c r="N105">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>240</v>
       </c>
@@ -5893,8 +6211,11 @@
       <c r="N106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>243</v>
       </c>
@@ -5937,8 +6258,11 @@
       <c r="N107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>245</v>
       </c>
@@ -5981,8 +6305,11 @@
       <c r="N108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O108">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>247</v>
       </c>
@@ -6025,8 +6352,11 @@
       <c r="N109">
         <v>2</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O109">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>249</v>
       </c>
@@ -6069,8 +6399,11 @@
       <c r="N110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>251</v>
       </c>
@@ -6113,8 +6446,11 @@
       <c r="N111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>253</v>
       </c>
@@ -6157,8 +6493,11 @@
       <c r="N112">
         <v>2</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>256</v>
       </c>
@@ -6201,8 +6540,11 @@
       <c r="N113">
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O113">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>258</v>
       </c>
@@ -6245,8 +6587,11 @@
       <c r="N114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>260</v>
       </c>
@@ -6289,8 +6634,11 @@
       <c r="N115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>262</v>
       </c>
@@ -6333,8 +6681,11 @@
       <c r="N116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>264</v>
       </c>
@@ -6377,8 +6728,11 @@
       <c r="N117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>266</v>
       </c>
@@ -6421,8 +6775,11 @@
       <c r="N118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>268</v>
       </c>
@@ -6465,8 +6822,11 @@
       <c r="N119">
         <v>3</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>270</v>
       </c>
@@ -6509,8 +6869,11 @@
       <c r="N120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>272</v>
       </c>
@@ -6553,8 +6916,11 @@
       <c r="N121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>274</v>
       </c>
@@ -6597,8 +6963,11 @@
       <c r="N122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>276</v>
       </c>
@@ -6641,8 +7010,11 @@
       <c r="N123">
         <v>4</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>278</v>
       </c>
@@ -6685,8 +7057,11 @@
       <c r="N124">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>280</v>
       </c>
@@ -6729,8 +7104,11 @@
       <c r="N125">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O125">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>282</v>
       </c>
@@ -6773,9 +7151,11 @@
       <c r="N126">
         <v>0</v>
       </c>
+      <c r="O126">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N126"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Against human mode, conditional spy placing added weight
</commit_message>
<xml_diff>
--- a/TUnderdark/Resources/Cards.xlsx
+++ b/TUnderdark/Resources/Cards.xlsx
@@ -9,20 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="12885"/>
+    <workbookView xWindow="4650" yWindow="0" windowWidth="27870" windowHeight="12885"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cards!$A$1:$N$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cards!$A$1:$Q$126</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="294">
   <si>
     <t>SpecificType</t>
   </si>
@@ -898,6 +898,12 @@
   </si>
   <si>
     <t>ReturnEnemySpy</t>
+  </si>
+  <si>
+    <t>IsPlaceSpyForEnemySpy</t>
+  </si>
+  <si>
+    <t>IsPlaceSpyForEnemyTroops</t>
   </si>
 </sst>
 </file>
@@ -1212,11 +1218,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O126"/>
+  <dimension ref="A1:Q126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N126" sqref="N126"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,7 +1239,7 @@
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1279,8 +1285,14 @@
       <c r="O1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1326,8 +1338,14 @@
       <c r="O2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1373,8 +1391,14 @@
       <c r="O3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1420,8 +1444,14 @@
       <c r="O4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1467,8 +1497,14 @@
       <c r="O5">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1514,8 +1550,14 @@
       <c r="O6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1561,8 +1603,14 @@
       <c r="O7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1608,8 +1656,14 @@
       <c r="O8">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P8" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1655,8 +1709,14 @@
       <c r="O9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P9" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1702,8 +1762,14 @@
       <c r="O10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P10" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1749,8 +1815,14 @@
       <c r="O11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P11" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1796,8 +1868,14 @@
       <c r="O12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P12" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1843,8 +1921,14 @@
       <c r="O13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1890,8 +1974,14 @@
       <c r="O14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P14" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1937,8 +2027,14 @@
       <c r="O15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P15" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1984,8 +2080,14 @@
       <c r="O16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2031,8 +2133,14 @@
       <c r="O17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -2078,8 +2186,14 @@
       <c r="O18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2125,8 +2239,14 @@
       <c r="O19">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2172,8 +2292,14 @@
       <c r="O20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2219,8 +2345,14 @@
       <c r="O21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P21" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2266,8 +2398,14 @@
       <c r="O22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P22" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2313,8 +2451,14 @@
       <c r="O23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P23" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -2360,8 +2504,14 @@
       <c r="O24">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2407,8 +2557,14 @@
       <c r="O25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P25" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2454,8 +2610,14 @@
       <c r="O26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P26" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -2501,8 +2663,14 @@
       <c r="O27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P27" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>66</v>
       </c>
@@ -2548,8 +2716,14 @@
       <c r="O28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P28" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>68</v>
       </c>
@@ -2595,8 +2769,14 @@
       <c r="O29">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P29" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -2642,8 +2822,14 @@
       <c r="O30">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P30" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>73</v>
       </c>
@@ -2689,8 +2875,14 @@
       <c r="O31">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P31" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -2736,8 +2928,14 @@
       <c r="O32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P32" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>77</v>
       </c>
@@ -2783,8 +2981,14 @@
       <c r="O33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P33" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2830,8 +3034,14 @@
       <c r="O34">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P34" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>81</v>
       </c>
@@ -2877,8 +3087,14 @@
       <c r="O35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P35" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2924,8 +3140,14 @@
       <c r="O36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P36" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -2971,8 +3193,14 @@
       <c r="O37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P37" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>89</v>
       </c>
@@ -3018,8 +3246,14 @@
       <c r="O38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P38" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>92</v>
       </c>
@@ -3065,8 +3299,14 @@
       <c r="O39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P39" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>94</v>
       </c>
@@ -3112,8 +3352,14 @@
       <c r="O40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P40" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>96</v>
       </c>
@@ -3159,8 +3405,14 @@
       <c r="O41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P41" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>98</v>
       </c>
@@ -3206,8 +3458,14 @@
       <c r="O42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P42" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>100</v>
       </c>
@@ -3253,8 +3511,14 @@
       <c r="O43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P43" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>102</v>
       </c>
@@ -3300,8 +3564,14 @@
       <c r="O44">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P44" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -3347,8 +3617,14 @@
       <c r="O45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P45" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>106</v>
       </c>
@@ -3394,8 +3670,14 @@
       <c r="O46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P46" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>109</v>
       </c>
@@ -3441,8 +3723,14 @@
       <c r="O47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P47" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -3488,8 +3776,14 @@
       <c r="O48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P48" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -3535,8 +3829,14 @@
       <c r="O49">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P49" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>115</v>
       </c>
@@ -3582,8 +3882,14 @@
       <c r="O50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P50" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>117</v>
       </c>
@@ -3629,8 +3935,14 @@
       <c r="O51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P51" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>119</v>
       </c>
@@ -3676,8 +3988,14 @@
       <c r="O52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P52" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>121</v>
       </c>
@@ -3723,8 +4041,14 @@
       <c r="O53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P53" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>124</v>
       </c>
@@ -3770,8 +4094,14 @@
       <c r="O54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P54" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>126</v>
       </c>
@@ -3817,8 +4147,14 @@
       <c r="O55">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P55" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>128</v>
       </c>
@@ -3864,8 +4200,14 @@
       <c r="O56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P56" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>130</v>
       </c>
@@ -3911,8 +4253,14 @@
       <c r="O57">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P57" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>133</v>
       </c>
@@ -3958,8 +4306,14 @@
       <c r="O58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P58" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>135</v>
       </c>
@@ -4005,8 +4359,14 @@
       <c r="O59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P59" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>137</v>
       </c>
@@ -4052,8 +4412,14 @@
       <c r="O60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P60" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>139</v>
       </c>
@@ -4099,8 +4465,14 @@
       <c r="O61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P61" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>141</v>
       </c>
@@ -4146,8 +4518,14 @@
       <c r="O62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P62" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>143</v>
       </c>
@@ -4193,8 +4571,14 @@
       <c r="O63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P63" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>145</v>
       </c>
@@ -4240,8 +4624,14 @@
       <c r="O64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P64" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>147</v>
       </c>
@@ -4287,8 +4677,14 @@
       <c r="O65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P65" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -4334,8 +4730,14 @@
       <c r="O66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P66" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>152</v>
       </c>
@@ -4381,8 +4783,14 @@
       <c r="O67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P67" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>154</v>
       </c>
@@ -4428,8 +4836,14 @@
       <c r="O68">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P68" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>156</v>
       </c>
@@ -4475,8 +4889,14 @@
       <c r="O69">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P69" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>158</v>
       </c>
@@ -4522,8 +4942,14 @@
       <c r="O70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P70" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>160</v>
       </c>
@@ -4569,8 +4995,14 @@
       <c r="O71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P71" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>162</v>
       </c>
@@ -4616,8 +5048,14 @@
       <c r="O72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P72" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>164</v>
       </c>
@@ -4663,8 +5101,14 @@
       <c r="O73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P73" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>166</v>
       </c>
@@ -4710,8 +5154,14 @@
       <c r="O74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P74" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>168</v>
       </c>
@@ -4757,8 +5207,14 @@
       <c r="O75">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P75" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>171</v>
       </c>
@@ -4804,8 +5260,14 @@
       <c r="O76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P76" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>174</v>
       </c>
@@ -4851,8 +5313,14 @@
       <c r="O77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P77" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>177</v>
       </c>
@@ -4898,8 +5366,14 @@
       <c r="O78">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P78" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>179</v>
       </c>
@@ -4945,8 +5419,14 @@
       <c r="O79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P79" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>181</v>
       </c>
@@ -4992,8 +5472,14 @@
       <c r="O80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P80" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>183</v>
       </c>
@@ -5039,8 +5525,14 @@
       <c r="O81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P81" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>185</v>
       </c>
@@ -5086,8 +5578,14 @@
       <c r="O82">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P82" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>188</v>
       </c>
@@ -5133,8 +5631,14 @@
       <c r="O83">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P83" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>190</v>
       </c>
@@ -5180,8 +5684,14 @@
       <c r="O84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P84" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>192</v>
       </c>
@@ -5227,8 +5737,14 @@
       <c r="O85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P85" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>194</v>
       </c>
@@ -5274,8 +5790,14 @@
       <c r="O86">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P86" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>196</v>
       </c>
@@ -5321,8 +5843,14 @@
       <c r="O87">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P87" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>199</v>
       </c>
@@ -5368,8 +5896,14 @@
       <c r="O88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P88" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>201</v>
       </c>
@@ -5415,8 +5949,14 @@
       <c r="O89">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P89" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>204</v>
       </c>
@@ -5462,8 +6002,14 @@
       <c r="O90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P90" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>206</v>
       </c>
@@ -5509,8 +6055,14 @@
       <c r="O91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P91" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>209</v>
       </c>
@@ -5556,8 +6108,14 @@
       <c r="O92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P92" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>212</v>
       </c>
@@ -5603,8 +6161,14 @@
       <c r="O93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P93" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q93" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>214</v>
       </c>
@@ -5650,8 +6214,14 @@
       <c r="O94">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P94" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>216</v>
       </c>
@@ -5697,8 +6267,14 @@
       <c r="O95">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P95" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>219</v>
       </c>
@@ -5744,8 +6320,14 @@
       <c r="O96">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P96" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>222</v>
       </c>
@@ -5791,8 +6373,14 @@
       <c r="O97">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P97" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>224</v>
       </c>
@@ -5838,8 +6426,14 @@
       <c r="O98">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P98" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>226</v>
       </c>
@@ -5885,8 +6479,14 @@
       <c r="O99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P99" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>228</v>
       </c>
@@ -5932,8 +6532,14 @@
       <c r="O100">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P100" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>230</v>
       </c>
@@ -5979,8 +6585,14 @@
       <c r="O101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P101" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>232</v>
       </c>
@@ -6026,8 +6638,14 @@
       <c r="O102">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P102" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>234</v>
       </c>
@@ -6073,8 +6691,14 @@
       <c r="O103">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P103" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>236</v>
       </c>
@@ -6120,8 +6744,14 @@
       <c r="O104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P104" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>238</v>
       </c>
@@ -6167,8 +6797,14 @@
       <c r="O105">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P105" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>240</v>
       </c>
@@ -6214,8 +6850,14 @@
       <c r="O106">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P106" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>243</v>
       </c>
@@ -6261,8 +6903,14 @@
       <c r="O107">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P107" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>245</v>
       </c>
@@ -6308,8 +6956,14 @@
       <c r="O108">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P108" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>247</v>
       </c>
@@ -6355,8 +7009,14 @@
       <c r="O109">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P109" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>249</v>
       </c>
@@ -6402,8 +7062,14 @@
       <c r="O110">
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P110" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>251</v>
       </c>
@@ -6449,8 +7115,14 @@
       <c r="O111">
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P111" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>253</v>
       </c>
@@ -6496,8 +7168,14 @@
       <c r="O112">
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P112" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>256</v>
       </c>
@@ -6543,8 +7221,14 @@
       <c r="O113">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P113" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>258</v>
       </c>
@@ -6590,8 +7274,14 @@
       <c r="O114">
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P114" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>260</v>
       </c>
@@ -6637,8 +7327,14 @@
       <c r="O115">
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P115" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>262</v>
       </c>
@@ -6684,8 +7380,14 @@
       <c r="O116">
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P116" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>264</v>
       </c>
@@ -6731,8 +7433,14 @@
       <c r="O117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P117" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q117" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>266</v>
       </c>
@@ -6778,8 +7486,14 @@
       <c r="O118">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P118" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>268</v>
       </c>
@@ -6825,8 +7539,14 @@
       <c r="O119">
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P119" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>270</v>
       </c>
@@ -6872,8 +7592,14 @@
       <c r="O120">
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P120" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>272</v>
       </c>
@@ -6919,8 +7645,14 @@
       <c r="O121">
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P121" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>274</v>
       </c>
@@ -6966,8 +7698,14 @@
       <c r="O122">
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P122" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>276</v>
       </c>
@@ -7013,8 +7751,14 @@
       <c r="O123">
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P123" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>278</v>
       </c>
@@ -7060,8 +7804,14 @@
       <c r="O124">
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P124" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>280</v>
       </c>
@@ -7107,8 +7857,14 @@
       <c r="O125">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P125" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>282</v>
       </c>
@@ -7154,8 +7910,15 @@
       <c r="O126">
         <v>0</v>
       </c>
+      <c r="P126" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q126" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q126"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>